<commit_message>
Change dotnet version to 4.5.2
</commit_message>
<xml_diff>
--- a/RegistrationFormGenerator/Assets/ExcelFormet.xlsx
+++ b/RegistrationFormGenerator/Assets/ExcelFormet.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Dept 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dept 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Dept 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="22">
   <si>
     <t>Serial</t>
   </si>
@@ -73,16 +73,25 @@
   </si>
   <si>
     <t>Admission Cancelled</t>
+  </si>
+  <si>
+    <t>Name 1</t>
+  </si>
+  <si>
+    <t>Eng name 1</t>
+  </si>
+  <si>
+    <t>..</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +129,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -166,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,9 +215,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,6 +250,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -407,15 +426,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
@@ -434,7 +453,7 @@
     <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,6 +513,68 @@
       </c>
       <c r="T1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -503,25 +584,189 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HTML Done Perfectly without image
</commit_message>
<xml_diff>
--- a/RegistrationFormGenerator/Assets/ExcelFormet.xlsx
+++ b/RegistrationFormGenerator/Assets/ExcelFormet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dept 1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="25">
   <si>
     <t>Serial</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Roll No</t>
   </si>
   <si>
-    <t>Session</t>
-  </si>
-  <si>
     <t>Father's Name (Bengali)</t>
   </si>
   <si>
@@ -82,6 +79,18 @@
   </si>
   <si>
     <t>..</t>
+  </si>
+  <si>
+    <t>DegeeNameBengali</t>
+  </si>
+  <si>
+    <t>DegeeNameEnglish</t>
+  </si>
+  <si>
+    <t>SessionBengali</t>
+  </si>
+  <si>
+    <t>SessionEnglish</t>
   </si>
 </sst>
 </file>
@@ -427,11 +436,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,18 +459,22 @@
     <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -473,108 +486,126 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
       <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
+      <c r="W1" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T2" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -585,10 +616,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,18 +817,22 @@
     <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -630,140 +844,126 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
       <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add debug info on error
</commit_message>
<xml_diff>
--- a/RegistrationFormGenerator/Assets/ExcelFormet.xlsx
+++ b/RegistrationFormGenerator/Assets/ExcelFormet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5BC3F941-5BA9-45DE-B7D0-6998EC51FB9A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DACB300-B447-4812-A6D1-03060A29898A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dept 1" sheetId="1" r:id="rId1"/>
@@ -133,18 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -493,9 +487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -693,7 +687,7 @@
     <col min="1" max="1" width="27.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -727,7 +721,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -801,7 +795,7 @@
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">

</xml_diff>